<commit_message>
Update SBTM Report Template v.1.1.xlsx
</commit_message>
<xml_diff>
--- a/Lab4/take-home/SBTM Report Template v.1.1.xlsx
+++ b/Lab4/take-home/SBTM Report Template v.1.1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="102">
   <si>
     <t>Last refreshed: Fri Apr 26 2024 00:40:37 GMT+0300 (Eastern European Summer Time).</t>
   </si>
@@ -814,11 +814,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1586844322"/>
-        <c:axId val="162446641"/>
+        <c:axId val="1856874741"/>
+        <c:axId val="65089754"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1586844322"/>
+        <c:axId val="1856874741"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -870,10 +870,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="162446641"/>
+        <c:crossAx val="65089754"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="162446641"/>
+        <c:axId val="65089754"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -948,7 +948,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1586844322"/>
+        <c:crossAx val="1856874741"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1070,11 +1070,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1839987538"/>
-        <c:axId val="1148082195"/>
+        <c:axId val="304198452"/>
+        <c:axId val="495799368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1839987538"/>
+        <c:axId val="304198452"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1126,10 +1126,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1148082195"/>
+        <c:crossAx val="495799368"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1148082195"/>
+        <c:axId val="495799368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1.0"/>
@@ -1205,7 +1205,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1839987538"/>
+        <c:crossAx val="304198452"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1538,12 +1538,8 @@
     </row>
     <row r="21">
       <c r="B21" s="15"/>
-      <c r="C21" s="15">
-        <v>1.0</v>
-      </c>
-      <c r="D21" s="15">
-        <v>0.0</v>
-      </c>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
       <c r="E21" s="15"/>
       <c r="H21" s="15" t="s">
         <v>27</v>
@@ -1574,12 +1570,7 @@
     </row>
     <row r="22">
       <c r="B22" s="9"/>
-      <c r="C22" s="15">
-        <v>1.0</v>
-      </c>
-      <c r="D22" s="15">
-        <v>0.0</v>
-      </c>
+      <c r="D22" s="15"/>
       <c r="E22" s="9"/>
       <c r="H22" s="15" t="s">
         <v>27</v>
@@ -1609,32 +1600,9 @@
       </c>
     </row>
     <row r="23">
-      <c r="H23" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="I23" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="J23" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="K23" s="16">
-        <v>45408.00213653935</v>
-      </c>
-      <c r="L23" s="9">
-        <v>0.55</v>
-      </c>
-      <c r="M23" s="9">
-        <v>2.0</v>
-      </c>
-      <c r="N23" s="17">
-        <f t="shared" ref="N23:O23" si="4">N22+L23</f>
-        <v>2.41</v>
-      </c>
-      <c r="O23" s="17">
-        <f t="shared" si="4"/>
-        <v>6</v>
-      </c>
+      <c r="K23" s="16"/>
+      <c r="N23" s="17"/>
+      <c r="O23" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>